<commit_message>
have .sql file for db backup
</commit_message>
<xml_diff>
--- a/project1/Data to input into DB/teacher data.xlsx
+++ b/project1/Data to input into DB/teacher data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boss\BeastCreatures\project1\Data to input into DB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="510" yWindow="570" windowWidth="14055" windowHeight="6090"/>
+    <workbookView xWindow="510" yWindow="1030" windowWidth="14060" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="127">
   <si>
     <t>first_name</t>
   </si>
@@ -251,12 +256,156 @@
   </si>
   <si>
     <t>Faculty id</t>
+  </si>
+  <si>
+    <t>English Composition</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+  </si>
+  <si>
+    <t>Discrete Math</t>
+  </si>
+  <si>
+    <t>Programming Language concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object Oriented Programming </t>
+  </si>
+  <si>
+    <t>Theory of Computation</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jean </t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Nauroto</t>
+  </si>
+  <si>
+    <t>Uzamaki</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Harden</t>
+  </si>
+  <si>
+    <t>Mohammad</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>teacher11</t>
+  </si>
+  <si>
+    <t>teacher12</t>
+  </si>
+  <si>
+    <t>teacher13</t>
+  </si>
+  <si>
+    <t>teacher14</t>
+  </si>
+  <si>
+    <t>teacher15</t>
+  </si>
+  <si>
+    <t>teacher16</t>
+  </si>
+  <si>
+    <t>teacher17</t>
+  </si>
+  <si>
+    <t>teacher18</t>
+  </si>
+  <si>
+    <t>teacher19</t>
+  </si>
+  <si>
+    <t>teacher20</t>
+  </si>
+  <si>
+    <t>parkerp2</t>
+  </si>
+  <si>
+    <t>waynep2</t>
+  </si>
+  <si>
+    <t>kentp2</t>
+  </si>
+  <si>
+    <t>grayp2</t>
+  </si>
+  <si>
+    <t>xavierp2</t>
+  </si>
+  <si>
+    <t>uzamakip2</t>
+  </si>
+  <si>
+    <t>hardenp2</t>
+  </si>
+  <si>
+    <t>alip2</t>
+  </si>
+  <si>
+    <t>pparker@google.com.au</t>
+  </si>
+  <si>
+    <t>bwayne7@yandex.ru</t>
+  </si>
+  <si>
+    <t>kclark12@free.fr</t>
+  </si>
+  <si>
+    <t>jgray8@jailbum.net</t>
+  </si>
+  <si>
+    <t>xcharly19@ihg.com</t>
+  </si>
+  <si>
+    <t>unauroto20@umich.edu</t>
+  </si>
+  <si>
+    <t>jharden@rambler.ru</t>
+  </si>
+  <si>
+    <t>amohamm@jailbum.net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -284,8 +433,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,6 +473,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -371,7 +524,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,9 +557,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,6 +609,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -615,25 +802,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -659,7 +846,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -685,7 +872,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -711,7 +898,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -737,7 +924,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -763,7 +950,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -789,7 +976,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -815,7 +1002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -841,7 +1028,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -867,7 +1054,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -893,7 +1080,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -917,6 +1104,236 @@
       </c>
       <c r="H11" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>